<commit_message>
Data table updates. PA system added
</commit_message>
<xml_diff>
--- a/XLSX/VVK_EIR_s3_NSIK_12_AS.xlsx
+++ b/XLSX/VVK_EIR_s3_NSIK_12_AS.xlsx
@@ -125,26 +125,26 @@
     <t xml:space="preserve">Tarp fiksuotų padėčių objektą ar objektus palaikantis komponentas, kuris įrengtas išilgai laikomojo komponento ar sistemos ir yra nuolatiniame sąlytyje su tuo komponentu ar sistema.</t>
   </si>
   <si>
-    <t xml:space="preserve">kabelio kopėčios, 
+    <t xml:space="preserve">vamzdžių dėklas, 
+laido kanalas, 
+vamzdžių kanalas, 
+kabelio kanalas, 
+įrangos laikiklis, 
+Kabelio kanalas, 
+kabelio lovelis, 
 įrangos dėklas, 
-Kabelio kanalas, 
-vamzdžių kanalas, 
-laido kanalas, 
+kabelių kanalas, 
+instaliacinis vamzdis, 
+kabelio vielinis lovelis, 
+įrenginių dėklas, 
+Atviras dėklas, 
 laidų dėklas, 
-kabelio lovelis, 
-kabelio kanalas, 
-vamzdžių dėklas, 
+kabelių laikiklis, 
+ryšio kabelių lovys, 
+uždaras dėklas, 
+kabelio kopėčios, 
 įrangą laikanti konstrukcija, 
-Atviras dėklas, 
-instaliacinis vamzdis, 
-kabelių kanalas, 
-įrenginių dėklas, 
-laidų kanalas, 
-uždaras dėklas, 
-įrangos laikiklis, 
-kabelio vielinis lovelis, 
-kabelių laikiklis, 
-ryšio kabelių lovys</t>
+laidų kanalas</t>
   </si>
   <si>
     <t xml:space="preserve">IfcFlowSegment, 
@@ -245,18 +245,18 @@
     <t xml:space="preserve">Elektrinis signalo apdorojimo komponentas, skirtas prietaisams valdyti be žmogaus įsikišimo.</t>
   </si>
   <si>
-    <t xml:space="preserve">Praėjimo vartelių Kontroleris, 
+    <t xml:space="preserve">sinchronizavimo relė, 
 Kontroleris, 
 Kortelių skaitytuvo kontroleris, 
+sinchronizatorius, 
+Durų kontroleris, 
+nuotolinis terminalas (RTU - angl. remote terminal unit), 
+Centrinis procesorius (CPU - angl. central processing unit), 
+nuotolinio televaldymo blokas (RTU - angl. remote telecontrol unit), 
+programuojamas loginis valdiklis (PLC - angl. programmable logic controller), 
 Valdiklis, 
-programuojamas loginis valdiklis (PLC - angl. programmable logic controller), 
-sinchronizatorius, 
-nuotolinio televaldymo blokas (RTU - angl. remote telecontrol unit), 
-Centrinis procesorius (CPU - angl. central processing unit), 
-sinchronizavimo relė, 
-Durų kontroleris, 
 nuotolinis apsaugos ir valdymo blokas, 
-nuotolinis terminalas (RTU - angl. remote terminal unit)</t>
+Praėjimo vartelių Kontroleris</t>
   </si>
   <si>
     <t xml:space="preserve">IfcDistributionControlElement, 
@@ -315,11 +315,11 @@
     <t xml:space="preserve">Sąveikos komponentas, valdomas spaudžiant pirštu.</t>
   </si>
   <si>
-    <t xml:space="preserve">Pavojaus mygtukas, 
+    <t xml:space="preserve">Klaviatūra, 
+klavišas, 
+Pavojaus mygtukas, 
 įspaudžiamas jungiklis, 
-įspaudžiamas mygtukas, 
-Klaviatūra, 
-klavišas</t>
+įspaudžiamas mygtukas</t>
   </si>
   <si>
     <t xml:space="preserve">IfcSensor, 
@@ -370,19 +370,19 @@
     <t xml:space="preserve">Gaubtas, skirtas mechanizmams ar jų dalims apsaugoti nuo išorinio poveikio bei užtikrinti žmonių saugumą (taip pat ir nuo kontakto su elektros srove).</t>
   </si>
   <si>
-    <t xml:space="preserve">saugos dėžutė, 
+    <t xml:space="preserve">Automatikos spinta, 
 spintelė, 
-elektros skydelis, 
+paskirstymo skydelis, 
+sensorių dėžutė, 
 montavimo dėžė, 
-sensorių dėžutė, 
-elektros spinta, 
 Prietaisų dėžė, 
 skydinė, 
+elektros spinta, 
 Centralė, 
+elektros skydelis, 
+saugos dėžutė, 
 kolektorių spintelė, 
-Automatikos spinta, 
-prietaisų dėžė, 
-paskirstymo skydelis</t>
+prietaisų dėžė</t>
   </si>
   <si>
     <t xml:space="preserve">Judesio daviklis</t>
@@ -413,8 +413,8 @@
   </si>
   <si>
     <t xml:space="preserve">Seisminis daviklis, 
-Seisminis jutiklis, 
-Smūgio daviklis</t>
+Smūgio daviklis, 
+Seisminis jutiklis</t>
   </si>
   <si>
     <t xml:space="preserve">Stiklo dūžio daviklis</t>
@@ -464,13 +464,13 @@
     <t xml:space="preserve">Spinduliuotės jutimo komponentas su skaliariniu išėjimu, skirtas neregimosioms elektromagnetinėms bangoms matuoti.</t>
   </si>
   <si>
-    <t xml:space="preserve">radarinis jutiklis, 
-Gama spinduliuotės detektorius, 
+    <t xml:space="preserve">Gama spinduliuotės detektorius, 
+UV jutiklis, 
 ir jutiklis, 
-ultravioletinių spindulių jutiklis, 
 Šiluminis daviklis, 
 infraraudonųjų spindulių jutiklis, 
-UV jutiklis</t>
+ultravioletinių spindulių jutiklis, 
+radarinis jutiklis</t>
   </si>
   <si>
     <t xml:space="preserve">Magnetinio lauko detektorius</t>
@@ -486,9 +486,9 @@
   </si>
   <si>
     <t xml:space="preserve">Magnetinis kontaktas, 
-herkonas, 
 Relė su sandariaisisias magnetiniais kontaktais, 
-sandarusis magnetinis jungiklis</t>
+sandarusis magnetinis jungiklis, 
+herkonas</t>
   </si>
   <si>
     <t xml:space="preserve">Garsiakalbis</t>
@@ -503,8 +503,8 @@
     <t xml:space="preserve">Judančios membranos principu veikiantis akustinis prietaisas.</t>
   </si>
   <si>
-    <t xml:space="preserve">sirena, 
-Garso kolonėlė, 
+    <t xml:space="preserve">Garso kolonėlė, 
+sirena, 
 Apsaugos signalizacijos blykstė</t>
   </si>
   <si>
@@ -550,13 +550,13 @@
     <t xml:space="preserve">Informacijos jutimo komponentas, naudojantis elektromagnetinį lauką.</t>
   </si>
   <si>
-    <t xml:space="preserve">radijo dažnio kortelės skaitytuvas (RFC - angl. radio frequency card), 
-magnetinės juostos skaitytuvas, 
+    <t xml:space="preserve">magnetinės juostos skaitytuvas, 
+RFC skaitytuvas, 
 RFID skaitytuvas, 
+radijo dažnio identifikavimo skaitytuvas (RFID - angl. radio frequency identification), 
+radijo dažnio kortelės skaitytuvas (RFC - angl. radio frequency card), 
 Nuotolinis kortelių skaitytuvas, 
-Juostos skaitytuvas, 
-radijo dažnio identifikavimo skaitytuvas (RFID - angl. radio frequency identification), 
-RFC skaitytuvas</t>
+Juostos skaitytuvas</t>
   </si>
   <si>
     <t xml:space="preserve">Skaitytuvai, nepatenkantys į RFID ir NFC technologijas</t>
@@ -604,12 +604,12 @@
     <t xml:space="preserve">Informacijos jutimo komponentas, naudojantis šviesą.</t>
   </si>
   <si>
-    <t xml:space="preserve">greito atsako kodo (QR - angl. quick responce) skaitytuvas, 
-QR kodų skeneris, 
+    <t xml:space="preserve">Akies rainelės skaitytuvas, 
+Brūkšninio kodo skaitytuvas, 
 optinio disko skaitytuvas, 
-Akies rainelės skaitytuvas, 
 QR skaitytuvas, 
-Brūkšninio kodo skaitytuvas</t>
+greito atsako kodo (QR - angl. quick responce) skaitytuvas, 
+QR kodų skeneris</t>
   </si>
   <si>
     <t xml:space="preserve">Lustų skaitytuvas</t>
@@ -624,9 +624,9 @@
     <t xml:space="preserve">Informacijos jutimo komponentas, naudojantis elektrinį sujungimą.</t>
   </si>
   <si>
-    <t xml:space="preserve">Dallas-key skaitytuvas, 
+    <t xml:space="preserve">Lustinės kortelės skaitytuvas, 
 Lustų skaitytuvas, 
-Lustinės kortelės skaitytuvas</t>
+Dallas-key skaitytuvas</t>
   </si>
   <si>
     <t xml:space="preserve">Elektromagnetas</t>
@@ -660,15 +660,15 @@
     <t xml:space="preserve">Vaizdinis garso ir vaizdo jutimo komponentas su skaliariniu išėjimu, skirtas regimajam vaizdui matuoti.</t>
   </si>
   <si>
-    <t xml:space="preserve">Kupolinė kamera, 
+    <t xml:space="preserve">uždaroji televizija (CCTV - angl. closed-circuit television), 
+Kamera, 
+Vaizdo kamera, 
+Valdoma kamera, 
+vaizdo kamera, 
+valdoma stebėjimo kamera (PTZ - angl. pan-tilt-zoom), 
 skeneris, 
-vaizdo kamera, 
-Kamera, 
-uždaroji televizija (CCTV - angl. closed-circuit television), 
-Vaizdo makera su pašvietimu, 
-Vaizdo kamera, 
-valdoma stebėjimo kamera (PTZ - angl. pan-tilt-zoom), 
-Valdoma kamera</t>
+Kupolinė kamera, 
+Vaizdo makera su pašvietimu</t>
   </si>
   <si>
     <t xml:space="preserve">Valdymo pultas</t>
@@ -683,11 +683,11 @@
     <t xml:space="preserve">Daugialypis interaktyvus įrenginys, apimantis rankines priemones.</t>
   </si>
   <si>
-    <t xml:space="preserve">žaidimų valdiklis, 
+    <t xml:space="preserve">Žaidimų konsolės įvesties įrenginys "joypad", 
+žaidimų skydelis, 
 PTZ pultas, 
-žaidimų skydelis, 
 Vaizdo kamerų valdymo pultas, 
-Žaidimų konsolės įvesties įrenginys "joypad"</t>
+žaidimų valdiklis</t>
   </si>
   <si>
     <t xml:space="preserve">Kortelių rašytuvas</t>
@@ -702,9 +702,9 @@
     <t xml:space="preserve">Elektrinio signalo apdorojimo komponentas, automatiškai išsaugantis kaupimo įrenginio įėjimo informaciją.</t>
   </si>
   <si>
-    <t xml:space="preserve">Juostos rašytuvas, 
-kompaktinių diskų rašytuvas, 
+    <t xml:space="preserve">kompaktinių diskų rašytuvas, 
 DVR, 
+Juostos rašytuvas, 
 optinių diskų rašytuvas, 
 Vaizdo įrašymo irenginys</t>
   </si>
@@ -743,20 +743,20 @@
 Duomenų paskirstymo panelė</t>
   </si>
   <si>
-    <t xml:space="preserve">saugos dėžutė, 
-spintelė, 
+    <t xml:space="preserve">spintelė, 
+paskirstymo skydelis, 
+sensorių dėžutė, 
+montavimo dėžė, 
+skydinė, 
+Centralė, 
+elektros skydelis, 
+elektros spinta, 
 Vaizdo kamerų dėžė, 
-elektros skydelis, 
-Centralė, 
-montavimo dėžė, 
+saugos dėžutė, 
+kolektorių spintelė, 
 Vaizdo kamerų sistemos spinta, 
-sensorių dėžutė, 
-elektros spinta, 
-skydinė, 
 Vaizdo kamerų sistemos įrenginių spinta, 
-kolektorių spintelė, 
-prietaisų dėžė, 
-paskirstymo skydelis</t>
+prietaisų dėžė</t>
   </si>
   <si>
     <t xml:space="preserve">Elektros skirstytuvas</t>
@@ -769,10 +769,10 @@
   </si>
   <si>
     <t xml:space="preserve">elektros šakotuvas, 
+Ilgintuvas, 
 Vaizdo kamerų sistemos elektros šakotuvas, 
 Elektros šakotuvas vaizdo kamerų sistemai, 
-"prailgintuvas", 
-Ilgintuvas</t>
+"prailgintuvas"</t>
   </si>
   <si>
     <t xml:space="preserve">Nepertraukiamo maitinimo šaltinis</t>
@@ -785,8 +785,8 @@
   </si>
   <si>
     <t xml:space="preserve">Vaizdo kamerų nepertraukiamo maitinimo šaltinis, 
-Vaizdo kamerų UPS, 
-UPS (angl. uninterrupted power supply)</t>
+UPS (angl. uninterrupted power supply), 
+Vaizdo kamerų UPS</t>
   </si>
   <si>
     <t xml:space="preserve">IfcElectricalElement, 
@@ -1327,7 +1327,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -1348,10 +1348,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="23" style="0" width="15"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="29" min="26" style="0" width="8.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="13.27"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="130.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="136.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>9</v>
@@ -15125,4 +15125,634 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentas" ma:contentTypeID="0x010100185EA42515F6E340ADA2406B64465806" ma:contentTypeVersion="21" ma:contentTypeDescription="Kurkite naują dokumentą." ma:contentTypeScope="" ma:versionID="69fce3456da530ef8df8c1288c92c649">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="68a813e2-ff10-41a8-84be-cc9e1093ee90" xmlns:ns3="1c51dfe2-a643-4496-b898-9dd06cb11735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6d7b953a17a9765602fbc16af246523" ns2:_="" ns3:_="">
+    <xsd:import namespace="68a813e2-ff10-41a8-84be-cc9e1093ee90"/>
+    <xsd:import namespace="1c51dfe2-a643-4496-b898-9dd06cb11735"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:Dokumentas" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxKeywordTaxHTField" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="68a813e2-ff10-41a8-84be-cc9e1093ee90" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Dokumentas" ma:index="13" nillable="true" ma:displayName="Dokumentas" ma:format="Hyperlink" ma:internalName="Dokumentas">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="26" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Vaizdų žymės" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="934a8a67-bd8a-4395-b6f5-189eb7ec8d86" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="27" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="28" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1c51dfe2-a643-4496-b898-9dd06cb11735" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Bendrinama su" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Bendrinta su išsamia informacija" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxKeywordTaxHTField" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="TaxKeywordTaxHTField" ma:taxonomyFieldName="TaxKeyword" ma:displayName="Įmonės raktažodžiai" ma:fieldId="{23f27201-bee3-471e-b2e7-b64fd8b7ca38}" ma:taxonomyMulti="true" ma:sspId="934a8a67-bd8a-4395-b6f5-189eb7ec8d86" ma:termSetId="00000000-0000-0000-0000-000000000000" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="true" ma:isKeyword="true">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="24" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{2909241f-a384-4ee9-b5bd-b403c264fad4}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="1c51dfe2-a643-4496-b898-9dd06cb11735">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Turinio tipas"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Antraštė"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxKeywordTaxHTField xmlns="1c51dfe2-a643-4496-b898-9dd06cb11735">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Dokumentas xmlns="68a813e2-ff10-41a8-84be-cc9e1093ee90">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Dokumentas>
+    <TaxCatchAll xmlns="1c51dfe2-a643-4496-b898-9dd06cb11735" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="68a813e2-ff10-41a8-84be-cc9e1093ee90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokumentas" ma:contentTypeID="0x010100185EA42515F6E340ADA2406B64465806" ma:contentTypeVersion="21" ma:contentTypeDescription="Kurkite naują dokumentą." ma:contentTypeScope="" ma:versionID="69fce3456da530ef8df8c1288c92c649">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="68a813e2-ff10-41a8-84be-cc9e1093ee90" xmlns:ns3="1c51dfe2-a643-4496-b898-9dd06cb11735" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6d7b953a17a9765602fbc16af246523" ns2:_="" ns3:_="">
+    <xsd:import namespace="68a813e2-ff10-41a8-84be-cc9e1093ee90"/>
+    <xsd:import namespace="1c51dfe2-a643-4496-b898-9dd06cb11735"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:Dokumentas" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxKeywordTaxHTField" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="68a813e2-ff10-41a8-84be-cc9e1093ee90" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Dokumentas" ma:index="13" nillable="true" ma:displayName="Dokumentas" ma:format="Hyperlink" ma:internalName="Dokumentas">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:URL">
+            <xsd:sequence>
+              <xsd:element name="Url" type="dms:ValidUrl" minOccurs="0" nillable="true"/>
+              <xsd:element name="Description" type="xsd:string" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="15" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="21" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="26" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Vaizdų žymės" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="934a8a67-bd8a-4395-b6f5-189eb7ec8d86" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="27" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="28" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1c51dfe2-a643-4496-b898-9dd06cb11735" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Bendrinama su" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Bendrinta su išsamia informacija" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxKeywordTaxHTField" ma:index="23" nillable="true" ma:taxonomy="true" ma:internalName="TaxKeywordTaxHTField" ma:taxonomyFieldName="TaxKeyword" ma:displayName="Įmonės raktažodžiai" ma:fieldId="{23f27201-bee3-471e-b2e7-b64fd8b7ca38}" ma:taxonomyMulti="true" ma:sspId="934a8a67-bd8a-4395-b6f5-189eb7ec8d86" ma:termSetId="00000000-0000-0000-0000-000000000000" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="true" ma:isKeyword="true">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="24" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{2909241f-a384-4ee9-b5bd-b403c264fad4}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="1c51dfe2-a643-4496-b898-9dd06cb11735">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Turinio tipas"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Antraštė"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Dokumentas xmlns="68a813e2-ff10-41a8-84be-cc9e1093ee90">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Dokumentas>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="68a813e2-ff10-41a8-84be-cc9e1093ee90">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c51dfe2-a643-4496-b898-9dd06cb11735" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="1c51dfe2-a643-4496-b898-9dd06cb11735">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9023426B-57E2-4EDC-8792-A85C6BB9BC06}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D930A1E5-B437-40DD-BCEC-41514F2C9DE9}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B765E045-84F7-4847-977D-A83CA7C1B4D2}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{146078EF-9712-4843-8DB4-8E08576C6A78}"/>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36078F14-2924-46B6-AB11-7D8436CAAEC2}"/>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53320421-1244-4032-BD23-FB2BB4E63E28}"/>
 </file>
</xml_diff>